<commit_message>
React router refresh problem fixed. Basename added to router in app.js
</commit_message>
<xml_diff>
--- a/src/backend/Untitled Form.xlsx
+++ b/src/backend/Untitled Form.xlsx
@@ -11,21 +11,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>Time Stamp</t>
   </si>
   <si>
-    <t>who is dumb?</t>
+    <t xml:space="preserve">Which is the capital city of Karnataka ? </t>
   </si>
   <si>
-    <t>Who am I?</t>
-  </si>
-  <si>
-    <t>Belgavi</t>
-  </si>
-  <si>
-    <t>Aditya</t>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -409,7 +403,8 @@
   <dimension ref="A1:C2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="3" width="12" customWidth="1"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="3" width="41" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -420,15 +415,12 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
+    <row r="2" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>